<commit_message>
removed non sense files
</commit_message>
<xml_diff>
--- a/reports/export-excel.xlsx
+++ b/reports/export-excel.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T36"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -444,25 +444,25 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Kèmi</v>
+        <v>Arielle Jémima Oyèmi</v>
       </c>
       <c r="B2" t="str">
-        <v>ABIOLA</v>
+        <v>ADJADOHOUN</v>
       </c>
       <c r="C2">
         <v>10000</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>50000</v>
+        <v>70000</v>
       </c>
       <c r="H2">
         <v>30000</v>
@@ -480,63 +480,63 @@
         <v>35000</v>
       </c>
       <c r="M2">
-        <v>20000</v>
+        <v>35000</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
-        <v>15000</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>35000</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>35000</v>
+        <v>30000</v>
       </c>
       <c r="T2">
-        <v>50000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Carmen</v>
+        <v>Sarè Obèd</v>
       </c>
       <c r="B3" t="str">
-        <v>ADDA</v>
+        <v>BIO</v>
       </c>
       <c r="C3">
         <v>10000</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="H3">
         <v>30000</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <v>35000</v>
@@ -563,21 +563,21 @@
         <v>35000</v>
       </c>
       <c r="T3">
-        <v>100000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Maïwenn Tiffany</v>
+        <v>Ossimar</v>
       </c>
       <c r="B4" t="str">
-        <v>AGAZOUNON</v>
+        <v>BOTOKOU</v>
       </c>
       <c r="C4">
         <v>10000</v>
       </c>
       <c r="D4">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -586,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>30000</v>
+        <v>100000</v>
       </c>
       <c r="H4">
         <v>30000</v>
@@ -604,51 +604,45 @@
         <v>35000</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
       <c r="O4">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="P4">
         <v>35000</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>70000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Amira</v>
+        <v>Ramdane</v>
       </c>
       <c r="B5" t="str">
-        <v>AKOBI ALASSANE</v>
+        <v>BOURAÏMA</v>
       </c>
       <c r="C5">
         <v>10000</v>
       </c>
       <c r="D5">
-        <v>5000</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="G5">
-        <v>30000</v>
+        <v>100000</v>
       </c>
       <c r="H5">
         <v>30000</v>
@@ -666,63 +660,63 @@
         <v>35000</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="P5">
         <v>35000</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>70000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Fertus</v>
+        <v>Eden Ange</v>
       </c>
       <c r="B6" t="str">
-        <v>AKPLOGAN KANHO</v>
+        <v>COCO</v>
       </c>
       <c r="C6">
         <v>10000</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="H6">
         <v>30000</v>
       </c>
       <c r="I6">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <v>35000</v>
@@ -749,30 +743,30 @@
         <v>35000</v>
       </c>
       <c r="T6">
-        <v>80000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Islène</v>
+        <v>Maéva Divine</v>
       </c>
       <c r="B7" t="str">
-        <v>AMOUSSOU</v>
+        <v>DECAKPOUEVOU</v>
       </c>
       <c r="C7">
         <v>10000</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>30000</v>
+        <v>70000</v>
       </c>
       <c r="H7">
         <v>30000</v>
@@ -790,51 +784,51 @@
         <v>35000</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="P7">
         <v>35000</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7">
-        <v>35000</v>
+        <v>30000</v>
       </c>
       <c r="T7">
-        <v>70000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Rogelyne</v>
+        <v>Sèna Happy Rébecca</v>
       </c>
       <c r="B8" t="str">
-        <v>ANANI</v>
+        <v>DOSSOU</v>
       </c>
       <c r="C8">
         <v>10000</v>
       </c>
       <c r="D8">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>95000</v>
+        <v>80000</v>
       </c>
       <c r="H8">
         <v>30000</v>
@@ -864,39 +858,39 @@
         <v>35000</v>
       </c>
       <c r="Q8">
-        <v>30000</v>
+        <v>15000</v>
       </c>
       <c r="R8">
         <v>0</v>
       </c>
       <c r="S8">
-        <v>5000</v>
+        <v>20000</v>
       </c>
       <c r="T8">
-        <v>5000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Ketia</v>
+        <v>Léo</v>
       </c>
       <c r="B9" t="str">
-        <v>AWESSOU</v>
+        <v>ETCHIN</v>
       </c>
       <c r="C9">
         <v>10000</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>30000</v>
+        <v>65000</v>
       </c>
       <c r="H9">
         <v>30000</v>
@@ -914,13 +908,13 @@
         <v>35000</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="N9">
         <v>0</v>
       </c>
       <c r="O9">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="P9">
         <v>35000</v>
@@ -935,30 +929,30 @@
         <v>35000</v>
       </c>
       <c r="T9">
-        <v>70000</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Malkiel</v>
+        <v>Leonel</v>
       </c>
       <c r="B10" t="str">
-        <v>AZONVIDE</v>
+        <v>ETCHIN</v>
       </c>
       <c r="C10">
         <v>10000</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>60000</v>
+        <v>65000</v>
       </c>
       <c r="H10">
         <v>30000</v>
@@ -976,13 +970,13 @@
         <v>35000</v>
       </c>
       <c r="M10">
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="N10">
         <v>0</v>
       </c>
       <c r="O10">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="P10">
         <v>35000</v>
@@ -997,92 +991,92 @@
         <v>35000</v>
       </c>
       <c r="T10">
-        <v>40000</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Adonis</v>
+        <v>Titilayo Emeraude Jacqueline</v>
       </c>
       <c r="B11" t="str">
-        <v>COMLAN</v>
+        <v>GBEDOLO</v>
       </c>
       <c r="C11">
         <v>10000</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G11">
+        <v>30000</v>
+      </c>
+      <c r="H11">
+        <v>30000</v>
+      </c>
+      <c r="I11">
+        <v>30000</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>35000</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>35000</v>
+      </c>
+      <c r="P11">
+        <v>35000</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>35000</v>
+      </c>
+      <c r="T11">
         <v>70000</v>
-      </c>
-      <c r="H11">
-        <v>30000</v>
-      </c>
-      <c r="I11">
-        <v>30000</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>35000</v>
-      </c>
-      <c r="M11">
-        <v>35000</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>35000</v>
-      </c>
-      <c r="Q11">
-        <v>5000</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>30000</v>
-      </c>
-      <c r="T11">
-        <v>30000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Princesse</v>
+        <v>Bryan Darren Férol</v>
       </c>
       <c r="B12" t="str">
-        <v>d'OLIVEIRA</v>
+        <v>GUEDEGBE</v>
       </c>
       <c r="C12">
         <v>10000</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>40000</v>
+        <v>65000</v>
       </c>
       <c r="H12">
         <v>30000</v>
@@ -1100,13 +1094,13 @@
         <v>35000</v>
       </c>
       <c r="M12">
-        <v>10000</v>
+        <v>35000</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
-        <v>25000</v>
+        <v>0</v>
       </c>
       <c r="P12">
         <v>35000</v>
@@ -1121,30 +1115,30 @@
         <v>35000</v>
       </c>
       <c r="T12">
-        <v>60000</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Honneur Josias</v>
+        <v>Axel</v>
       </c>
       <c r="B13" t="str">
-        <v>DOHOUE</v>
+        <v xml:space="preserve">HOUNSOU </v>
       </c>
       <c r="C13">
         <v>10000</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>65000</v>
+        <v>50000</v>
       </c>
       <c r="H13">
         <v>30000</v>
@@ -1162,13 +1156,13 @@
         <v>35000</v>
       </c>
       <c r="M13">
-        <v>35000</v>
+        <v>20000</v>
       </c>
       <c r="N13">
         <v>0</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="P13">
         <v>35000</v>
@@ -1183,30 +1177,30 @@
         <v>35000</v>
       </c>
       <c r="T13">
-        <v>35000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Jeanne D'Arc</v>
+        <v>Merveille Fèmi</v>
       </c>
       <c r="B14" t="str">
-        <v>DOSSOU</v>
+        <v>IGUE</v>
       </c>
       <c r="C14">
         <v>10000</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>50000</v>
+        <v>70000</v>
       </c>
       <c r="H14">
         <v>30000</v>
@@ -1224,63 +1218,63 @@
         <v>35000</v>
       </c>
       <c r="M14">
-        <v>20000</v>
+        <v>35000</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
-        <v>15000</v>
+        <v>0</v>
       </c>
       <c r="P14">
         <v>35000</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="R14">
         <v>0</v>
       </c>
       <c r="S14">
-        <v>35000</v>
+        <v>30000</v>
       </c>
       <c r="T14">
-        <v>50000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Koffi David</v>
+        <v>Evan</v>
       </c>
       <c r="B15" t="str">
-        <v>DOTSE</v>
+        <v>KOULO</v>
       </c>
       <c r="C15">
         <v>10000</v>
       </c>
       <c r="D15">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <v>30000</v>
       </c>
       <c r="I15">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="L15">
         <v>35000</v>
@@ -1307,30 +1301,30 @@
         <v>35000</v>
       </c>
       <c r="T15">
-        <v>70000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Coffi G. Laurex</v>
+        <v>Osnel</v>
       </c>
       <c r="B16" t="str">
-        <v>GNACADJA</v>
+        <v>KPADJOUDA</v>
       </c>
       <c r="C16">
         <v>10000</v>
       </c>
       <c r="D16">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>65000</v>
+        <v>100000</v>
       </c>
       <c r="H16">
         <v>30000</v>
@@ -1360,24 +1354,24 @@
         <v>35000</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="R16">
         <v>0</v>
       </c>
       <c r="S16">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <v>35000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Shalom David</v>
+        <v>Sènan Marie Vianney</v>
       </c>
       <c r="B17" t="str">
-        <v>GUEDEGBE</v>
+        <v>PATENON</v>
       </c>
       <c r="C17">
         <v>10000</v>
@@ -1392,31 +1386,31 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>20000</v>
+        <v>55000</v>
       </c>
       <c r="H17">
         <v>30000</v>
       </c>
       <c r="I17">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
       <c r="K17">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="L17">
         <v>35000</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="N17">
         <v>0</v>
       </c>
       <c r="O17">
-        <v>35000</v>
+        <v>10000</v>
       </c>
       <c r="P17">
         <v>35000</v>
@@ -1431,15 +1425,15 @@
         <v>35000</v>
       </c>
       <c r="T17">
-        <v>80000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Précieux</v>
+        <v>Jean Eudes</v>
       </c>
       <c r="B18" t="str">
-        <v>GUENDEHOU</v>
+        <v>PEREIRA</v>
       </c>
       <c r="C18">
         <v>10000</v>
@@ -1454,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>65000</v>
+        <v>30000</v>
       </c>
       <c r="H18">
         <v>30000</v>
@@ -1472,13 +1466,13 @@
         <v>35000</v>
       </c>
       <c r="M18">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="N18">
         <v>0</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="P18">
         <v>35000</v>
@@ -1493,24 +1487,30 @@
         <v>35000</v>
       </c>
       <c r="T18">
-        <v>35000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Grâce</v>
+        <v>Korédélé Ayouba</v>
       </c>
       <c r="B19" t="str">
-        <v>HOUNKPONOU</v>
+        <v>SALAHOU</v>
       </c>
       <c r="C19">
         <v>10000</v>
       </c>
       <c r="D19">
+        <v>10000</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>70000</v>
+        <v>50000</v>
       </c>
       <c r="H19">
         <v>30000</v>
@@ -1528,51 +1528,51 @@
         <v>35000</v>
       </c>
       <c r="M19">
-        <v>35000</v>
+        <v>20000</v>
       </c>
       <c r="N19">
         <v>0</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="P19">
         <v>35000</v>
       </c>
       <c r="Q19">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
       <c r="S19">
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="T19">
-        <v>30000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Sean</v>
+        <v>Aristide Jason</v>
       </c>
       <c r="B20" t="str">
-        <v>HOUNTONDJI</v>
+        <v>SECLOKA</v>
       </c>
       <c r="C20">
         <v>10000</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>100000</v>
+        <v>65000</v>
       </c>
       <c r="H20">
         <v>30000</v>
@@ -1602,39 +1602,39 @@
         <v>35000</v>
       </c>
       <c r="Q20">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="R20">
         <v>0</v>
       </c>
       <c r="S20">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Olayèmi Luderic</v>
+        <v>Djimefa Admirelle Irina</v>
       </c>
       <c r="B21" t="str">
-        <v>KEGBE</v>
+        <v>SOGLO</v>
       </c>
       <c r="C21">
         <v>10000</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>30000</v>
+        <v>55000</v>
       </c>
       <c r="H21">
         <v>30000</v>
@@ -1652,13 +1652,13 @@
         <v>35000</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="N21">
         <v>0</v>
       </c>
       <c r="O21">
-        <v>35000</v>
+        <v>10000</v>
       </c>
       <c r="P21">
         <v>35000</v>
@@ -1673,15 +1673,15 @@
         <v>35000</v>
       </c>
       <c r="T21">
-        <v>70000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Ihechi Hanniel</v>
+        <v>Fructueux</v>
       </c>
       <c r="B22" t="str">
-        <v>KOUKOUI</v>
+        <v>YEMIHIN</v>
       </c>
       <c r="C22">
         <v>10000</v>
@@ -1696,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>65000</v>
+        <v>40000</v>
       </c>
       <c r="H22">
         <v>30000</v>
@@ -1714,13 +1714,13 @@
         <v>35000</v>
       </c>
       <c r="M22">
-        <v>35000</v>
+        <v>10000</v>
       </c>
       <c r="N22">
         <v>0</v>
       </c>
       <c r="O22">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="P22">
         <v>35000</v>
@@ -1735,880 +1735,12 @@
         <v>35000</v>
       </c>
       <c r="T22">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v xml:space="preserve"> Candice Loriane</v>
-      </c>
-      <c r="B23" t="str">
-        <v>KOUSSOUHON</v>
-      </c>
-      <c r="C23">
-        <v>10000</v>
-      </c>
-      <c r="D23">
-        <v>10000</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
         <v>60000</v>
-      </c>
-      <c r="H23">
-        <v>30000</v>
-      </c>
-      <c r="I23">
-        <v>30000</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>35000</v>
-      </c>
-      <c r="M23">
-        <v>30000</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>5000</v>
-      </c>
-      <c r="P23">
-        <v>35000</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <v>35000</v>
-      </c>
-      <c r="T23">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="str">
-        <v>Jéhobène Marianique Akpédjé</v>
-      </c>
-      <c r="B24" t="str">
-        <v>KPALETE</v>
-      </c>
-      <c r="C24">
-        <v>10000</v>
-      </c>
-      <c r="D24">
-        <v>10000</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>70000</v>
-      </c>
-      <c r="H24">
-        <v>30000</v>
-      </c>
-      <c r="I24">
-        <v>30000</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>35000</v>
-      </c>
-      <c r="M24">
-        <v>35000</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>35000</v>
-      </c>
-      <c r="Q24">
-        <v>5000</v>
-      </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
-      <c r="S24">
-        <v>30000</v>
-      </c>
-      <c r="T24">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="str">
-        <v>Doriane</v>
-      </c>
-      <c r="B25" t="str">
-        <v>KPASSELOKOHINTO</v>
-      </c>
-      <c r="C25">
-        <v>10000</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>10000</v>
-      </c>
-      <c r="G25">
-        <v>70000</v>
-      </c>
-      <c r="H25">
-        <v>30000</v>
-      </c>
-      <c r="I25">
-        <v>30000</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>35000</v>
-      </c>
-      <c r="M25">
-        <v>35000</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <v>35000</v>
-      </c>
-      <c r="Q25">
-        <v>5000</v>
-      </c>
-      <c r="R25">
-        <v>0</v>
-      </c>
-      <c r="S25">
-        <v>30000</v>
-      </c>
-      <c r="T25">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>Esdras Donald</v>
-      </c>
-      <c r="B26" t="str">
-        <v>LOKOSSOU</v>
-      </c>
-      <c r="C26">
-        <v>10000</v>
-      </c>
-      <c r="D26">
-        <v>10000</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>60000</v>
-      </c>
-      <c r="H26">
-        <v>30000</v>
-      </c>
-      <c r="I26">
-        <v>30000</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>35000</v>
-      </c>
-      <c r="M26">
-        <v>30000</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <v>5000</v>
-      </c>
-      <c r="P26">
-        <v>35000</v>
-      </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26">
-        <v>0</v>
-      </c>
-      <c r="S26">
-        <v>35000</v>
-      </c>
-      <c r="T26">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>Haschem</v>
-      </c>
-      <c r="B27" t="str">
-        <v>MAMA ABDOU</v>
-      </c>
-      <c r="C27">
-        <v>10000</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>10000</v>
-      </c>
-      <c r="G27">
-        <v>25000</v>
-      </c>
-      <c r="H27">
-        <v>30000</v>
-      </c>
-      <c r="I27">
-        <v>25000</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>5000</v>
-      </c>
-      <c r="L27">
-        <v>35000</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="O27">
-        <v>35000</v>
-      </c>
-      <c r="P27">
-        <v>35000</v>
-      </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
-      <c r="S27">
-        <v>35000</v>
-      </c>
-      <c r="T27">
-        <v>75000</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="str">
-        <v>Riskiyath</v>
-      </c>
-      <c r="B28" t="str">
-        <v>SALIFOU</v>
-      </c>
-      <c r="C28">
-        <v>10000</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>10000</v>
-      </c>
-      <c r="G28">
-        <v>30000</v>
-      </c>
-      <c r="H28">
-        <v>30000</v>
-      </c>
-      <c r="I28">
-        <v>30000</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>35000</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
-      <c r="O28">
-        <v>35000</v>
-      </c>
-      <c r="P28">
-        <v>35000</v>
-      </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
-      <c r="S28">
-        <v>35000</v>
-      </c>
-      <c r="T28">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="str">
-        <v>Sarah</v>
-      </c>
-      <c r="B29" t="str">
-        <v>SASSOU</v>
-      </c>
-      <c r="C29">
-        <v>10000</v>
-      </c>
-      <c r="D29">
-        <v>10000</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>55000</v>
-      </c>
-      <c r="H29">
-        <v>30000</v>
-      </c>
-      <c r="I29">
-        <v>30000</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>35000</v>
-      </c>
-      <c r="M29">
-        <v>25000</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <v>10000</v>
-      </c>
-      <c r="P29">
-        <v>35000</v>
-      </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-      <c r="R29">
-        <v>0</v>
-      </c>
-      <c r="S29">
-        <v>35000</v>
-      </c>
-      <c r="T29">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="str">
-        <v>Ifè</v>
-      </c>
-      <c r="B30" t="str">
-        <v>SEDE</v>
-      </c>
-      <c r="C30">
-        <v>10000</v>
-      </c>
-      <c r="D30">
-        <v>10000</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>30000</v>
-      </c>
-      <c r="H30">
-        <v>30000</v>
-      </c>
-      <c r="I30">
-        <v>30000</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <v>35000</v>
-      </c>
-      <c r="M30">
-        <v>0</v>
-      </c>
-      <c r="N30">
-        <v>0</v>
-      </c>
-      <c r="O30">
-        <v>35000</v>
-      </c>
-      <c r="P30">
-        <v>35000</v>
-      </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
-      <c r="R30">
-        <v>0</v>
-      </c>
-      <c r="S30">
-        <v>35000</v>
-      </c>
-      <c r="T30">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="str">
-        <v>Rosvaldo</v>
-      </c>
-      <c r="B31" t="str">
-        <v>SOGLAGBE</v>
-      </c>
-      <c r="C31">
-        <v>10000</v>
-      </c>
-      <c r="D31">
-        <v>10000</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>40000</v>
-      </c>
-      <c r="H31">
-        <v>30000</v>
-      </c>
-      <c r="I31">
-        <v>30000</v>
-      </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>35000</v>
-      </c>
-      <c r="M31">
-        <v>10000</v>
-      </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <v>25000</v>
-      </c>
-      <c r="P31">
-        <v>35000</v>
-      </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
-      <c r="R31">
-        <v>0</v>
-      </c>
-      <c r="S31">
-        <v>35000</v>
-      </c>
-      <c r="T31">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="str">
-        <v>Kelyan</v>
-      </c>
-      <c r="B32" t="str">
-        <v>TOSSOU</v>
-      </c>
-      <c r="C32">
-        <v>10000</v>
-      </c>
-      <c r="D32">
-        <v>10000</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>50000</v>
-      </c>
-      <c r="H32">
-        <v>30000</v>
-      </c>
-      <c r="I32">
-        <v>30000</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <v>35000</v>
-      </c>
-      <c r="M32">
-        <v>20000</v>
-      </c>
-      <c r="N32">
-        <v>0</v>
-      </c>
-      <c r="O32">
-        <v>15000</v>
-      </c>
-      <c r="P32">
-        <v>35000</v>
-      </c>
-      <c r="Q32">
-        <v>0</v>
-      </c>
-      <c r="R32">
-        <v>0</v>
-      </c>
-      <c r="S32">
-        <v>35000</v>
-      </c>
-      <c r="T32">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="str">
-        <v>Archange Leroi</v>
-      </c>
-      <c r="B33" t="str">
-        <v>VLETIEN</v>
-      </c>
-      <c r="C33">
-        <v>10000</v>
-      </c>
-      <c r="D33">
-        <v>10000</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>60000</v>
-      </c>
-      <c r="H33">
-        <v>30000</v>
-      </c>
-      <c r="I33">
-        <v>30000</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-      <c r="L33">
-        <v>35000</v>
-      </c>
-      <c r="M33">
-        <v>30000</v>
-      </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
-      <c r="O33">
-        <v>5000</v>
-      </c>
-      <c r="P33">
-        <v>35000</v>
-      </c>
-      <c r="Q33">
-        <v>0</v>
-      </c>
-      <c r="R33">
-        <v>0</v>
-      </c>
-      <c r="S33">
-        <v>35000</v>
-      </c>
-      <c r="T33">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="str">
-        <v>Magnificat</v>
-      </c>
-      <c r="B34" t="str">
-        <v>VODOUNOU</v>
-      </c>
-      <c r="C34">
-        <v>10000</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>10000</v>
-      </c>
-      <c r="G34">
-        <v>50000</v>
-      </c>
-      <c r="H34">
-        <v>30000</v>
-      </c>
-      <c r="I34">
-        <v>30000</v>
-      </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-      <c r="L34">
-        <v>35000</v>
-      </c>
-      <c r="M34">
-        <v>20000</v>
-      </c>
-      <c r="N34">
-        <v>0</v>
-      </c>
-      <c r="O34">
-        <v>15000</v>
-      </c>
-      <c r="P34">
-        <v>35000</v>
-      </c>
-      <c r="Q34">
-        <v>0</v>
-      </c>
-      <c r="R34">
-        <v>0</v>
-      </c>
-      <c r="S34">
-        <v>35000</v>
-      </c>
-      <c r="T34">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="str">
-        <v>Kiyane</v>
-      </c>
-      <c r="B35" t="str">
-        <v>YESSOUF</v>
-      </c>
-      <c r="C35">
-        <v>10000</v>
-      </c>
-      <c r="D35">
-        <v>5000</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>5000</v>
-      </c>
-      <c r="G35">
-        <v>100000</v>
-      </c>
-      <c r="H35">
-        <v>30000</v>
-      </c>
-      <c r="I35">
-        <v>30000</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <v>35000</v>
-      </c>
-      <c r="M35">
-        <v>35000</v>
-      </c>
-      <c r="N35">
-        <v>0</v>
-      </c>
-      <c r="O35">
-        <v>0</v>
-      </c>
-      <c r="P35">
-        <v>35000</v>
-      </c>
-      <c r="Q35">
-        <v>35000</v>
-      </c>
-      <c r="R35">
-        <v>0</v>
-      </c>
-      <c r="S35">
-        <v>0</v>
-      </c>
-      <c r="T35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="str">
-        <v>Marie Annaelle</v>
-      </c>
-      <c r="B36" t="str">
-        <v>ZINZINDOHOUE</v>
-      </c>
-      <c r="C36">
-        <v>10000</v>
-      </c>
-      <c r="D36">
-        <v>10000</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>30000</v>
-      </c>
-      <c r="H36">
-        <v>30000</v>
-      </c>
-      <c r="I36">
-        <v>30000</v>
-      </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36">
-        <v>35000</v>
-      </c>
-      <c r="M36">
-        <v>0</v>
-      </c>
-      <c r="N36">
-        <v>0</v>
-      </c>
-      <c r="O36">
-        <v>35000</v>
-      </c>
-      <c r="P36">
-        <v>35000</v>
-      </c>
-      <c r="Q36">
-        <v>0</v>
-      </c>
-      <c r="R36">
-        <v>0</v>
-      </c>
-      <c r="S36">
-        <v>35000</v>
-      </c>
-      <c r="T36">
-        <v>70000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:T36"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:T22"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>